<commit_message>
[ADR-2614] update alns requirements
</commit_message>
<xml_diff>
--- a/alns/src/main/kotlin/output/output.xlsx
+++ b/alns/src/main/kotlin/output/output.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="43">
   <si>
     <t>Staff</t>
   </si>
@@ -110,22 +110,16 @@
     <t>A1</t>
   </si>
   <si>
-    <t>DO</t>
-  </si>
-  <si>
-    <t>PH</t>
-  </si>
-  <si>
     <t>M3</t>
   </si>
   <si>
+    <t>Staff_2</t>
+  </si>
+  <si>
+    <t>M2</t>
+  </si>
+  <si>
     <t>A2</t>
-  </si>
-  <si>
-    <t>M2</t>
-  </si>
-  <si>
-    <t>Staff_2</t>
   </si>
   <si>
     <t>Staff_3</t>
@@ -297,19 +291,19 @@
         <v>30</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G2" t="s" s="0">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H2" t="s" s="0">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I2" t="s" s="0">
         <v>30</v>
@@ -318,58 +312,58 @@
         <v>32</v>
       </c>
       <c r="K2" t="s" s="0">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L2" t="s" s="0">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="M2" t="s" s="0">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="N2" t="s" s="0">
         <v>31</v>
       </c>
       <c r="O2" t="s" s="0">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="P2" t="s" s="0">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="Q2" t="s" s="0">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="R2" t="s" s="0">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="S2" t="s" s="0">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="T2" t="s" s="0">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="U2" t="s" s="0">
         <v>31</v>
       </c>
       <c r="V2" t="s" s="0">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="W2" t="s" s="0">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="X2" t="s" s="0">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="Y2" t="s" s="0">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="Z2" t="s" s="0">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="AA2" t="s" s="0">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AB2" t="s" s="0">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AC2" t="s" s="0">
         <v>30</v>
@@ -377,10 +371,10 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s" s="0">
         <v>32</v>
@@ -389,242 +383,242 @@
         <v>30</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G3" t="s" s="0">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H3" t="s" s="0">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="I3" t="s" s="0">
         <v>30</v>
       </c>
       <c r="J3" t="s" s="0">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K3" t="s" s="0">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="L3" t="s" s="0">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="M3" t="s" s="0">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="N3" t="s" s="0">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="O3" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="P3" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Q3" t="s" s="0">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="R3" t="s" s="0">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="S3" t="s" s="0">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="T3" t="s" s="0">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="U3" t="s" s="0">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="V3" t="s" s="0">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="W3" t="s" s="0">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="X3" t="s" s="0">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="Y3" t="s" s="0">
         <v>34</v>
       </c>
       <c r="Z3" t="s" s="0">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AA3" t="s" s="0">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="AB3" t="s" s="0">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="AC3" t="s" s="0">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F4" t="s" s="0">
         <v>30</v>
       </c>
       <c r="G4" t="s" s="0">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="H4" t="s" s="0">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="I4" t="s" s="0">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J4" t="s" s="0">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="K4" t="s" s="0">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L4" t="s" s="0">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="M4" t="s" s="0">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="N4" t="s" s="0">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="O4" t="s" s="0">
         <v>30</v>
       </c>
       <c r="P4" t="s" s="0">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q4" t="s" s="0">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="R4" t="s" s="0">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="S4" t="s" s="0">
         <v>32</v>
       </c>
       <c r="T4" t="s" s="0">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="U4" t="s" s="0">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="V4" t="s" s="0">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="W4" t="s" s="0">
         <v>30</v>
       </c>
       <c r="X4" t="s" s="0">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="Y4" t="s" s="0">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Z4" t="s" s="0">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="AA4" t="s" s="0">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AB4" t="s" s="0">
         <v>31</v>
       </c>
       <c r="AC4" t="s" s="0">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s" s="0">
         <v>32</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F5" t="s" s="0">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G5" t="s" s="0">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="H5" t="s" s="0">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="I5" t="s" s="0">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J5" t="s" s="0">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K5" t="s" s="0">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="L5" t="s" s="0">
         <v>32</v>
       </c>
       <c r="M5" t="s" s="0">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="N5" t="s" s="0">
         <v>35</v>
       </c>
       <c r="O5" t="s" s="0">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="P5" t="s" s="0">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q5" t="s" s="0">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="R5" t="s" s="0">
         <v>30</v>
       </c>
       <c r="S5" t="s" s="0">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="T5" t="s" s="0">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="U5" t="s" s="0">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="V5" t="s" s="0">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="W5" t="s" s="0">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="X5" t="s" s="0">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="Y5" t="s" s="0">
         <v>34</v>
@@ -639,45 +633,45 @@
         <v>31</v>
       </c>
       <c r="AC5" t="s" s="0">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s" s="0">
         <v>30</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E6" t="s" s="0">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F6" t="s" s="0">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="G6" t="s" s="0">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H6" t="s" s="0">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I6" t="s" s="0">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="J6" t="s" s="0">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K6" t="s" s="0">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="L6" t="s" s="0">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="M6" t="s" s="0">
         <v>34</v>
@@ -692,99 +686,99 @@
         <v>30</v>
       </c>
       <c r="Q6" t="s" s="0">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="R6" t="s" s="0">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="S6" t="s" s="0">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="T6" t="s" s="0">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="U6" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="V6" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="W6" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="X6" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="Y6" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="Z6" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="AA6" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="AB6" t="s" s="0">
         <v>35</v>
       </c>
-      <c r="V6" t="s" s="0">
-        <v>35</v>
-      </c>
-      <c r="W6" t="s" s="0">
-        <v>30</v>
-      </c>
-      <c r="X6" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="Y6" t="s" s="0">
-        <v>35</v>
-      </c>
-      <c r="Z6" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="AA6" t="s" s="0">
-        <v>35</v>
-      </c>
-      <c r="AB6" t="s" s="0">
-        <v>31</v>
-      </c>
       <c r="AC6" t="s" s="0">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s" s="0">
         <v>30</v>
       </c>
       <c r="C7" t="s" s="0">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D7" t="s" s="0">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E7" t="s" s="0">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F7" t="s" s="0">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G7" t="s" s="0">
         <v>31</v>
       </c>
       <c r="H7" t="s" s="0">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I7" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J7" t="s" s="0">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="K7" t="s" s="0">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L7" t="s" s="0">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="M7" t="s" s="0">
         <v>30</v>
       </c>
       <c r="N7" t="s" s="0">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="O7" t="s" s="0">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="P7" t="s" s="0">
         <v>30</v>
       </c>
       <c r="Q7" t="s" s="0">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="R7" t="s" s="0">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="S7" t="s" s="0">
         <v>32</v>
@@ -796,25 +790,25 @@
         <v>31</v>
       </c>
       <c r="V7" t="s" s="0">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="W7" t="s" s="0">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="X7" t="s" s="0">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="Y7" t="s" s="0">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="Z7" t="s" s="0">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="AA7" t="s" s="0">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="AB7" t="s" s="0">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="AC7" t="s" s="0">
         <v>30</v>
@@ -822,123 +816,123 @@
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s" s="0">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s" s="0">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E8" t="s" s="0">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F8" t="s" s="0">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G8" t="s" s="0">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H8" t="s" s="0">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="I8" t="s" s="0">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="J8" t="s" s="0">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K8" t="s" s="0">
         <v>30</v>
       </c>
       <c r="L8" t="s" s="0">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="M8" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="N8" t="s" s="0">
         <v>35</v>
       </c>
-      <c r="N8" t="s" s="0">
-        <v>34</v>
-      </c>
       <c r="O8" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="P8" t="s" s="0">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q8" t="s" s="0">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="R8" t="s" s="0">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="S8" t="s" s="0">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="T8" t="s" s="0">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="U8" t="s" s="0">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="V8" t="s" s="0">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="W8" t="s" s="0">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="X8" t="s" s="0">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="Y8" t="s" s="0">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="Z8" t="s" s="0">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="AA8" t="s" s="0">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="AB8" t="s" s="0">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="AC8" t="s" s="0">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9" t="s" s="0">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D9" t="s" s="0">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E9" t="s" s="0">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F9" t="s" s="0">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G9" t="s" s="0">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H9" t="s" s="0">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I9" t="s" s="0">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="J9" t="s" s="0">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K9" t="s" s="0">
         <v>30</v>
@@ -947,84 +941,84 @@
         <v>32</v>
       </c>
       <c r="M9" t="s" s="0">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N9" t="s" s="0">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="O9" t="s" s="0">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="P9" t="s" s="0">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q9" t="s" s="0">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="R9" t="s" s="0">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="S9" t="s" s="0">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="T9" t="s" s="0">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="U9" t="s" s="0">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="V9" t="s" s="0">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="W9" t="s" s="0">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="X9" t="s" s="0">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="Y9" t="s" s="0">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="Z9" t="s" s="0">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="AA9" t="s" s="0">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="AB9" t="s" s="0">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="AC9" t="s" s="0">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s" s="0">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D10" t="s" s="0">
         <v>32</v>
       </c>
       <c r="E10" t="s" s="0">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F10" t="s" s="0">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G10" t="s" s="0">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="H10" t="s" s="0">
         <v>34</v>
       </c>
       <c r="I10" t="s" s="0">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="J10" t="s" s="0">
         <v>30</v>
@@ -1033,58 +1027,58 @@
         <v>34</v>
       </c>
       <c r="L10" t="s" s="0">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="M10" t="s" s="0">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N10" t="s" s="0">
         <v>31</v>
       </c>
       <c r="O10" t="s" s="0">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P10" t="s" s="0">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q10" t="s" s="0">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="R10" t="s" s="0">
         <v>32</v>
       </c>
       <c r="S10" t="s" s="0">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="T10" t="s" s="0">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="U10" t="s" s="0">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="V10" t="s" s="0">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="W10" t="s" s="0">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="X10" t="s" s="0">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="Y10" t="s" s="0">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Z10" t="s" s="0">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="AA10" t="s" s="0">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="AB10" t="s" s="0">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="AC10" t="s" s="0">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>